<commit_message>
Rebuild Finance templates with correct industry content - 25 templates updated/added
</commit_message>
<xml_diff>
--- a/static/templates/Finance_Change_Management_Plan.xlsx
+++ b/static/templates/Finance_Change_Management_Plan.xlsx
@@ -557,7 +557,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>FINANCE Change Management Plan Project</t>
+          <t>Banking Implementation Project</t>
         </is>
       </c>
     </row>
@@ -584,7 +584,7 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>Enterprise AI/ML Implementation</t>
+          <t>Enterprise Banking Implementation</t>
         </is>
       </c>
     </row>
@@ -660,6 +660,7 @@
         </is>
       </c>
     </row>
+    <row r="13"/>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
@@ -670,7 +671,7 @@
     <row r="15">
       <c r="A15" s="5" t="inlineStr">
         <is>
-          <t>1. Achieve 95% user adoption of new AI/ML systems within 6 months of go-live</t>
+          <t>1. Achieve 95% user adoption of new Banking systems within 6 months of go-live</t>
         </is>
       </c>
       <c r="B15" s="6" t="n"/>
@@ -698,7 +699,7 @@
     <row r="17">
       <c r="A17" s="5" t="inlineStr">
         <is>
-          <t>3. Build organizational capability and confidence in AI/ML technologies</t>
+          <t>3. Build organizational capability and confidence in Banking technologies</t>
         </is>
       </c>
       <c r="B17" s="6" t="n"/>
@@ -740,7 +741,7 @@
     <row r="20">
       <c r="A20" s="5" t="inlineStr">
         <is>
-          <t>6. Create positive stakeholder sentiment and enthusiasm for AI/ML transformation</t>
+          <t>6. Create positive stakeholder sentiment and enthusiasm for Banking transformation</t>
         </is>
       </c>
       <c r="B20" s="6" t="n"/>
@@ -751,6 +752,7 @@
       <c r="G20" s="6" t="n"/>
       <c r="H20" s="7" t="n"/>
     </row>
+    <row r="21"/>
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
@@ -902,6 +904,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" s="9" t="inlineStr">
         <is>
@@ -995,7 +998,7 @@
       </c>
       <c r="G4" s="5" t="inlineStr">
         <is>
-          <t>AI/ML automation</t>
+          <t>Banking automation</t>
         </is>
       </c>
       <c r="H4" s="5" t="inlineStr">
@@ -1737,6 +1740,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" s="9" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
RESTORE: Recover all 973 original multi-industry template files from commit 168d9c4
</commit_message>
<xml_diff>
--- a/static/templates/Finance_Change_Management_Plan.xlsx
+++ b/static/templates/Finance_Change_Management_Plan.xlsx
@@ -557,7 +557,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Banking Implementation Project</t>
+          <t>FINANCE Change Management Plan Project</t>
         </is>
       </c>
     </row>
@@ -584,7 +584,7 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>Enterprise Banking Implementation</t>
+          <t>Enterprise AI/ML Implementation</t>
         </is>
       </c>
     </row>
@@ -660,7 +660,6 @@
         </is>
       </c>
     </row>
-    <row r="13"/>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
@@ -671,7 +670,7 @@
     <row r="15">
       <c r="A15" s="5" t="inlineStr">
         <is>
-          <t>1. Achieve 95% user adoption of new Banking systems within 6 months of go-live</t>
+          <t>1. Achieve 95% user adoption of new AI/ML systems within 6 months of go-live</t>
         </is>
       </c>
       <c r="B15" s="6" t="n"/>
@@ -699,7 +698,7 @@
     <row r="17">
       <c r="A17" s="5" t="inlineStr">
         <is>
-          <t>3. Build organizational capability and confidence in Banking technologies</t>
+          <t>3. Build organizational capability and confidence in AI/ML technologies</t>
         </is>
       </c>
       <c r="B17" s="6" t="n"/>
@@ -741,7 +740,7 @@
     <row r="20">
       <c r="A20" s="5" t="inlineStr">
         <is>
-          <t>6. Create positive stakeholder sentiment and enthusiasm for Banking transformation</t>
+          <t>6. Create positive stakeholder sentiment and enthusiasm for AI/ML transformation</t>
         </is>
       </c>
       <c r="B20" s="6" t="n"/>
@@ -752,7 +751,6 @@
       <c r="G20" s="6" t="n"/>
       <c r="H20" s="7" t="n"/>
     </row>
-    <row r="21"/>
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
@@ -904,7 +902,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" s="9" t="inlineStr">
         <is>
@@ -998,7 +995,7 @@
       </c>
       <c r="G4" s="5" t="inlineStr">
         <is>
-          <t>Banking automation</t>
+          <t>AI/ML automation</t>
         </is>
       </c>
       <c r="H4" s="5" t="inlineStr">
@@ -1740,7 +1737,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" s="9" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Revert "RESTORE: Recover all 973 original multi-industry template files from commit 168d9c4"
This reverts commit 34e0294628a300884912c81167183ac88d5638c9.
</commit_message>
<xml_diff>
--- a/static/templates/Finance_Change_Management_Plan.xlsx
+++ b/static/templates/Finance_Change_Management_Plan.xlsx
@@ -557,7 +557,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>FINANCE Change Management Plan Project</t>
+          <t>Banking Implementation Project</t>
         </is>
       </c>
     </row>
@@ -584,7 +584,7 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>Enterprise AI/ML Implementation</t>
+          <t>Enterprise Banking Implementation</t>
         </is>
       </c>
     </row>
@@ -660,6 +660,7 @@
         </is>
       </c>
     </row>
+    <row r="13"/>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
@@ -670,7 +671,7 @@
     <row r="15">
       <c r="A15" s="5" t="inlineStr">
         <is>
-          <t>1. Achieve 95% user adoption of new AI/ML systems within 6 months of go-live</t>
+          <t>1. Achieve 95% user adoption of new Banking systems within 6 months of go-live</t>
         </is>
       </c>
       <c r="B15" s="6" t="n"/>
@@ -698,7 +699,7 @@
     <row r="17">
       <c r="A17" s="5" t="inlineStr">
         <is>
-          <t>3. Build organizational capability and confidence in AI/ML technologies</t>
+          <t>3. Build organizational capability and confidence in Banking technologies</t>
         </is>
       </c>
       <c r="B17" s="6" t="n"/>
@@ -740,7 +741,7 @@
     <row r="20">
       <c r="A20" s="5" t="inlineStr">
         <is>
-          <t>6. Create positive stakeholder sentiment and enthusiasm for AI/ML transformation</t>
+          <t>6. Create positive stakeholder sentiment and enthusiasm for Banking transformation</t>
         </is>
       </c>
       <c r="B20" s="6" t="n"/>
@@ -751,6 +752,7 @@
       <c r="G20" s="6" t="n"/>
       <c r="H20" s="7" t="n"/>
     </row>
+    <row r="21"/>
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
@@ -902,6 +904,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" s="9" t="inlineStr">
         <is>
@@ -995,7 +998,7 @@
       </c>
       <c r="G4" s="5" t="inlineStr">
         <is>
-          <t>AI/ML automation</t>
+          <t>Banking automation</t>
         </is>
       </c>
       <c r="H4" s="5" t="inlineStr">
@@ -1737,6 +1740,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" s="9" t="inlineStr">
         <is>

</xml_diff>